<commit_message>
Soil and Methane Samples
</commit_message>
<xml_diff>
--- a/CH4/Soil Inventory Ecuador Update.xlsx
+++ b/CH4/Soil Inventory Ecuador Update.xlsx
@@ -467,13 +467,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97:F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>